<commit_message>
add export buttons for measurement program
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,7 +450,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1.4154</v>
+        <v>0.5693</v>
       </c>
     </row>
     <row r="3">
@@ -458,7 +458,7 @@
         <v>0.25</v>
       </c>
       <c r="B3" t="n">
-        <v>1.4959</v>
+        <v>1.1853</v>
       </c>
     </row>
     <row r="4">
@@ -466,7 +466,7 @@
         <v>0.5</v>
       </c>
       <c r="B4" t="n">
-        <v>1.5515</v>
+        <v>1.5019</v>
       </c>
     </row>
     <row r="5">
@@ -474,7 +474,7 @@
         <v>0.75</v>
       </c>
       <c r="B5" t="n">
-        <v>1.5921</v>
+        <v>1.5628</v>
       </c>
     </row>
     <row r="6">
@@ -482,7 +482,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="n">
-        <v>1.62</v>
+        <v>1.6132</v>
       </c>
     </row>
     <row r="7">
@@ -490,7 +490,7 @@
         <v>1.25</v>
       </c>
       <c r="B7" t="n">
-        <v>1.6455</v>
+        <v>1.641</v>
       </c>
     </row>
     <row r="8">
@@ -498,7 +498,7 @@
         <v>1.5</v>
       </c>
       <c r="B8" t="n">
-        <v>1.6704</v>
+        <v>1.6643</v>
       </c>
     </row>
     <row r="9">
@@ -506,111 +506,7 @@
         <v>1.75</v>
       </c>
       <c r="B9" t="n">
-        <v>1.6929</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>2</v>
-      </c>
-      <c r="B10" t="n">
-        <v>1.7147</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>2.25</v>
-      </c>
-      <c r="B11" t="n">
-        <v>1.7365</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="B12" t="n">
-        <v>1.7576</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>2.75</v>
-      </c>
-      <c r="B13" t="n">
-        <v>1.7779</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>3</v>
-      </c>
-      <c r="B14" t="n">
-        <v>1.7982</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>3.25</v>
-      </c>
-      <c r="B15" t="n">
-        <v>1.8178</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="B16" t="n">
-        <v>1.8373</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>3.75</v>
-      </c>
-      <c r="B17" t="n">
-        <v>1.8576</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>4</v>
-      </c>
-      <c r="B18" t="n">
-        <v>1.8772</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>4.25</v>
-      </c>
-      <c r="B19" t="n">
-        <v>1.896</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="B20" t="n">
-        <v>1.9155</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>4.75</v>
-      </c>
-      <c r="B21" t="n">
-        <v>1.9343</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="n">
-        <v>5</v>
-      </c>
-      <c r="B22" t="n">
-        <v>1.9531</v>
+        <v>1.6877</v>
       </c>
     </row>
   </sheetData>

</xml_diff>